<commit_message>
The Scene And Player Readin Logic
</commit_message>
<xml_diff>
--- a/Src/Assets/Common/Tables/Tables/ActionDefine.xlsx
+++ b/Src/Assets/Common/Tables/Tables/ActionDefine.xlsx
@@ -5,10 +5,10 @@
   <workbookPr updateLinks="always" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Game-maker\1-NewClap\CCA\Src\Clap\Assets\Common\Tables\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Game-maker\0_CCA_new\Src\Assets\Common\Tables\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C59AC86-02FE-4DBB-A9AB-D19DAD7CAB53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CC742A-2CB5-4274-9B88-97821BF56C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="599" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="105">
   <si>
     <t>ID</t>
   </si>
@@ -114,23 +114,7 @@
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>Supply</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
     <t>Enemy</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>Attack</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>Defend</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>Counter</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
@@ -367,10 +351,6 @@
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>laser_overclocked_apocalypse</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
     <t>鬼斩</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
@@ -407,14 +387,6 @@
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
   <si>
-    <t>severance_parry</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
-    <t>御斩</t>
-    <phoneticPr fontId="15" type="noConversion"/>
-  </si>
-  <si>
     <t>rebounce</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
@@ -440,6 +412,18 @@
   </si>
   <si>
     <t>comeon</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>laser_cannon</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>deflect</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>偏折</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
@@ -732,7 +716,7 @@
     <cellStyle name="好 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
     <cellStyle name="适中 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="31">
     <dxf>
       <font>
         <sz val="9"/>
@@ -821,26 +805,6 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.992828150273141E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
@@ -902,26 +866,6 @@
         <patternFill patternType="none"/>
       </fill>
       <alignment horizontal="center" vertical="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.992828150273141E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <font>
@@ -1042,26 +986,6 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.992828150273141E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
@@ -1169,26 +1093,6 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-4.992828150273141E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
         <outline val="0"/>
@@ -1266,53 +1170,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A1:I5" totalsRowShown="0">
-  <autoFilter ref="A1:I5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Key" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ID" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="32"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Description" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{D2B0378F-2AC7-48BB-B226-76242E6C2C82}" name="Costs" dataDxfId="30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表1" displayName="表1" ref="A1:H5" totalsRowShown="0">
+  <autoFilter ref="A1:H5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Key" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="ID" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="28"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Description" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{D2B0378F-2AC7-48BB-B226-76242E6C2C82}" name="Costs" dataDxfId="26"/>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="TargetType"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="ItemType" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{D39F3B12-7181-4342-830A-9DA34F8EF285}" name="CD" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{B346CB5C-591C-4832-AA88-E75EBEBACD7E}" name="SupplyNumber" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{D39F3B12-7181-4342-830A-9DA34F8EF285}" name="CD" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{B346CB5C-591C-4832-AA88-E75EBEBACD7E}" name="SupplyNumber" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6AAE696F-C7CE-4533-8F63-E9BDB46E5712}" name="表1_3" displayName="表1_3" ref="A1:J14" totalsRowShown="0">
-  <autoFilter ref="A1:J14" xr:uid="{6AAE696F-C7CE-4533-8F63-E9BDB46E5712}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{F3120D7C-A45E-4FA2-B5BE-40DA2E6B527D}" name="Key" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{DACBB893-CA05-4D02-85D5-4BD88763CDC8}" name="ID" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{E05E1824-9A14-47F2-A1F4-06305E7C3F01}" name="Name" dataDxfId="24"/>
-    <tableColumn id="24" xr3:uid="{05C56AEC-8EEB-4DC5-90D4-589693695F9F}" name="Description" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{ECB0F01F-2D12-43FF-88D0-8932B311B9C3}" name="Costs" dataDxfId="22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6AAE696F-C7CE-4533-8F63-E9BDB46E5712}" name="表1_3" displayName="表1_3" ref="A1:I14" totalsRowShown="0">
+  <autoFilter ref="A1:I14" xr:uid="{6AAE696F-C7CE-4533-8F63-E9BDB46E5712}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{F3120D7C-A45E-4FA2-B5BE-40DA2E6B527D}" name="Key" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{DACBB893-CA05-4D02-85D5-4BD88763CDC8}" name="ID" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{E05E1824-9A14-47F2-A1F4-06305E7C3F01}" name="Name" dataDxfId="21"/>
+    <tableColumn id="24" xr3:uid="{05C56AEC-8EEB-4DC5-90D4-589693695F9F}" name="Description" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{ECB0F01F-2D12-43FF-88D0-8932B311B9C3}" name="Costs" dataDxfId="19"/>
     <tableColumn id="11" xr3:uid="{8738C2BC-B1DC-4B88-A546-C9264D49325B}" name="TargetType"/>
-    <tableColumn id="25" xr3:uid="{7F7BFBB1-E753-41AC-903C-5D0048E4A48B}" name="ItemType" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{A4A2D2D8-BA27-47D8-82A1-4708B0912A01}" name="CD" dataDxfId="20"/>
-    <tableColumn id="27" xr3:uid="{C523F30B-8528-475C-AB56-584489F12893}" name="Level" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{9F4863C8-14DF-490F-AAED-DA9CA6CCA3A6}" name="Damage" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{A4A2D2D8-BA27-47D8-82A1-4708B0912A01}" name="CD" dataDxfId="18"/>
+    <tableColumn id="27" xr3:uid="{C523F30B-8528-475C-AB56-584489F12893}" name="Level" dataDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{9F4863C8-14DF-490F-AAED-DA9CA6CCA3A6}" name="Damage" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BBDA416B-0922-4AAF-A799-D524740B3D14}" name="表1_4" displayName="表1_4" ref="A1:H5" totalsRowShown="0">
-  <autoFilter ref="A1:H5" xr:uid="{BBDA416B-0922-4AAF-A799-D524740B3D14}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{BE94463F-5F58-4AE5-8D3C-9ED629948C9E}" name="Key" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{65052D3C-90DB-42DF-8C3A-74AA612BEF48}" name="ID" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{2510B181-E22D-4568-AC36-382E43DA1F65}" name="Name" dataDxfId="15"/>
-    <tableColumn id="24" xr3:uid="{4BE18853-2496-4AA4-942D-324B9DDFB7C9}" name="Description" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{002F1A29-9EEC-44DB-A228-41BEF0AE2B11}" name="Costs" dataDxfId="13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BBDA416B-0922-4AAF-A799-D524740B3D14}" name="表1_4" displayName="表1_4" ref="A1:G5" totalsRowShown="0">
+  <autoFilter ref="A1:G5" xr:uid="{BBDA416B-0922-4AAF-A799-D524740B3D14}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{BE94463F-5F58-4AE5-8D3C-9ED629948C9E}" name="Key" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{65052D3C-90DB-42DF-8C3A-74AA612BEF48}" name="ID" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{2510B181-E22D-4568-AC36-382E43DA1F65}" name="Name" dataDxfId="13"/>
+    <tableColumn id="24" xr3:uid="{4BE18853-2496-4AA4-942D-324B9DDFB7C9}" name="Description" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{002F1A29-9EEC-44DB-A228-41BEF0AE2B11}" name="Costs" dataDxfId="11"/>
     <tableColumn id="11" xr3:uid="{45609FCE-4413-4353-9C89-BD89EFDE4C5D}" name="TargetType"/>
-    <tableColumn id="25" xr3:uid="{DB0C709A-B019-493D-AD85-3BBA6DC70451}" name="ItemType" dataDxfId="12"/>
     <tableColumn id="4" xr3:uid="{3D0100FB-1F43-427C-8534-CDC24303D7E6}" name="CD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1320,16 +1221,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B3284A1-AA19-4A39-984C-72F0ECC55A5D}" name="表1_45" displayName="表1_45" ref="A1:H5" totalsRowShown="0">
-  <autoFilter ref="A1:H5" xr:uid="{8B3284A1-AA19-4A39-984C-72F0ECC55A5D}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{A1AF415F-7938-4DF8-BACD-2F3931097179}" name="Key" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{0F312E1F-9C3E-4D2C-9F68-C6E87C1EE718}" name="ID" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{B5C76171-0265-42F6-8D5B-4662AAE7F83A}" name="Name" dataDxfId="9"/>
-    <tableColumn id="24" xr3:uid="{25AD89C3-2F76-4593-98BE-A3775460F142}" name="Description" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00DA4CE3-ED05-49B6-9190-58A0333EB78C}" name="Costs" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8B3284A1-AA19-4A39-984C-72F0ECC55A5D}" name="表1_45" displayName="表1_45" ref="A1:G5" totalsRowShown="0">
+  <autoFilter ref="A1:G5" xr:uid="{8B3284A1-AA19-4A39-984C-72F0ECC55A5D}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{A1AF415F-7938-4DF8-BACD-2F3931097179}" name="Key" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{0F312E1F-9C3E-4D2C-9F68-C6E87C1EE718}" name="ID" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{B5C76171-0265-42F6-8D5B-4662AAE7F83A}" name="Name" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{25AD89C3-2F76-4593-98BE-A3775460F142}" name="Description" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00DA4CE3-ED05-49B6-9190-58A0333EB78C}" name="Costs" dataDxfId="6"/>
     <tableColumn id="11" xr3:uid="{E2FEB15A-3782-40F3-A1CA-89D1DDC325AD}" name="TargetType"/>
-    <tableColumn id="25" xr3:uid="{45F084DB-6AAA-426A-96AF-4A75F9196759}" name="ItemType" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{688FFF09-C71B-441C-B52A-14B5A669665E}" name="CD"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1641,10 +1541,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.26953125" defaultRowHeight="14.5"/>
@@ -1654,14 +1554,13 @@
     <col min="3" max="3" width="12.90625" style="1" customWidth="1"/>
     <col min="4" max="5" width="14.36328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.81640625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="16.26953125" style="2"/>
-    <col min="11" max="16384" width="16.26953125" style="2"/>
+    <col min="7" max="8" width="16.26953125" style="2"/>
+    <col min="10" max="16384" width="16.26953125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1673,28 +1572,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="15">
+      <c r="G1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>6</v>
@@ -1703,58 +1599,52 @@
         <v>7</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" ht="15">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="1:10" ht="15">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>9</v>
@@ -1763,51 +1653,45 @@
         <v>10</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="15">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="2"/>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -1821,10 +1705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27ECECD7-19E1-4627-A931-18B44035B88A}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1834,12 +1718,12 @@
     <col min="3" max="3" width="10.6328125" customWidth="1"/>
     <col min="4" max="4" width="46.6328125" customWidth="1"/>
     <col min="5" max="5" width="18.26953125" customWidth="1"/>
-    <col min="9" max="9" width="9.54296875" customWidth="1"/>
+    <col min="8" max="8" width="9.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1851,435 +1735,393 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15">
+      <c r="G1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15">
       <c r="A2" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="5">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5">
         <v>2</v>
       </c>
-      <c r="J2" s="6">
+      <c r="I2" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:9" ht="15">
       <c r="A3" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>3</v>
       </c>
       <c r="I3" s="6">
-        <v>3</v>
-      </c>
-      <c r="J3" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:9" ht="15">
       <c r="A4" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>2</v>
       </c>
       <c r="I4" s="6">
         <v>2</v>
       </c>
-      <c r="J4" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15">
+    </row>
+    <row r="5" spans="1:9" ht="15">
       <c r="A5" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3</v>
       </c>
       <c r="I5" s="6">
-        <v>3</v>
-      </c>
-      <c r="J5" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>5</v>
       </c>
       <c r="I6" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15">
+      <c r="A7" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
         <v>5</v>
       </c>
-      <c r="J6" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15">
-      <c r="A7" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
       <c r="I7" s="6">
-        <v>5</v>
-      </c>
-      <c r="J7" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15">
+    <row r="8" spans="1:9" ht="15">
       <c r="A8" s="13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>4</v>
       </c>
       <c r="I8" s="6">
-        <v>4</v>
-      </c>
-      <c r="J8" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15">
+    <row r="9" spans="1:9" ht="15">
       <c r="A9" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>4</v>
       </c>
       <c r="I9" s="6">
-        <v>4</v>
-      </c>
-      <c r="J9" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15">
+    <row r="10" spans="1:9" ht="15">
       <c r="A10" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="12">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>4</v>
+      </c>
+      <c r="I10" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15">
+      <c r="A11" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" ht="15">
+      <c r="A12" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>6</v>
+      </c>
+      <c r="I12" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15">
+      <c r="A13" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="12">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>4</v>
-      </c>
-      <c r="J10" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15">
-      <c r="A11" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1</v>
-      </c>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" ht="15">
-      <c r="A12" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="6">
+      <c r="E13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
         <v>6</v>
       </c>
-      <c r="J12" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
       <c r="I13" s="6">
-        <v>6</v>
-      </c>
-      <c r="J13" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15">
+    <row r="14" spans="1:9" ht="15">
       <c r="A14" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>7</v>
       </c>
       <c r="I14" s="6">
-        <v>7</v>
-      </c>
-      <c r="J14" s="6">
         <v>3</v>
       </c>
     </row>
@@ -2295,10 +2137,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2886CEDB-A2BB-4C5C-B7C0-8A8D819EC72C}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2308,9 +2150,9 @@
     <col min="4" max="4" width="48.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2322,119 +2164,104 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15">
+      <c r="G1" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15">
       <c r="A2" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15">
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15">
       <c r="A3" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15">
       <c r="A4" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15">
       <c r="A5" s="13" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5">
+      <c r="G5">
         <v>0</v>
       </c>
     </row>
@@ -2450,10 +2277,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FC6B873-DDE4-475A-AF60-FACC4E0D297A}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2464,9 +2291,9 @@
     <col min="5" max="5" width="10.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2478,128 +2305,113 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15">
+      <c r="G1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15">
       <c r="A2" s="13" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2" s="11"/>
-    </row>
-    <row r="3" spans="1:9" ht="15">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" ht="15">
       <c r="A3" s="13" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" ht="15">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4" s="11"/>
-    </row>
-    <row r="5" spans="1:9" ht="15">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="13" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="11"/>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -2615,7 +2427,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2629,7 +2441,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15">
       <c r="A1" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -2638,10 +2450,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -2655,25 +2467,25 @@
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="13" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>28</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="H2" s="6">
         <v>1</v>
@@ -2681,25 +2493,25 @@
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="13" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="H3" s="6">
         <v>1</v>

</xml_diff>